<commit_message>
add chart for IZI041 dataset
</commit_message>
<xml_diff>
--- a/Data/IZI041_20250320-133102.xlsx
+++ b/Data/IZI041_20250320-133102.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B3A63D-0D9C-4FB6-8A04-6D8D91922213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FCD446-AE2D-4B45-8EDF-DA7AB938DF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="9">
   <si>
     <t>Pavisam</t>
   </si>
@@ -71,12 +71,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,7 +104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +407,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,46 +423,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D1" s="4">
+      <c r="D1" s="1">
         <v>2011</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="1">
         <v>2012</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="1">
         <v>2013</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="1">
         <v>2014</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="1">
         <v>2015</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="1">
         <v>2016</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="1">
         <v>2017</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="1">
         <v>2018</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="1">
         <v>2019</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="1">
         <v>2020</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="1">
         <v>2021</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O1" s="1">
         <v>2022</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="1">
         <v>2023</v>
       </c>
-      <c r="Q1" s="4">
+      <c r="Q1" s="1">
         <v>2024</v>
       </c>
     </row>
@@ -469,288 +476,318 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>19.100000000000001</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>17.2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>15.6</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>15.2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>13.8</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="4">
         <v>13.3</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="4">
         <v>12.3</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="4">
         <v>11.6</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="4">
         <v>10.3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>11.9</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>12.1</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="4">
         <v>11.3</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="4">
         <v>10</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="4">
         <v>10.7</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>16</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>14.9</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>13</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>12</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>10.5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>11.2</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="4">
         <v>10.3</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="4">
         <v>7.8</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="4">
         <v>7.9</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>7.1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>8.6</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="4">
         <v>8.6</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="4">
         <v>7.2</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>24.9</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>21.2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>19.7</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>19.899999999999999</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>18.399999999999999</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>16.100000000000001</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>15.1</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>16.8</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>13.8</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>19.5</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="4">
         <v>18</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="4">
         <v>16.5</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="4">
         <v>16.100000000000001</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="4">
         <v>14.6</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>16.100000000000001</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>14.1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>14.2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>12.5</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="4">
         <v>11.2</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="4">
         <v>10.3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="4">
         <v>9.5</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>8.1</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>11.1</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>10</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="4">
         <v>10.8</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="4">
         <v>9.9</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="4">
         <v>10.9</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>15.7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>13.6</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>11.7</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>10.5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="4">
         <v>6.3</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="4">
         <v>6.3</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
         <v>6.7</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="4">
         <v>7.1</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="4">
         <v>8.5</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="4">
         <v>7</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="4">
         <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>24.2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>17.7</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>19.2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>16.7</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="4">
         <v>13.7</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="4">
         <v>12.8</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>13.8</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="4">
         <v>10.7</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>18</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>14.8</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="4">
         <v>15.1</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="4">
         <v>16</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="4">
         <v>15.9</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -801,6 +838,12 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -848,6 +891,12 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
@@ -948,6 +997,12 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
@@ -995,6 +1050,12 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1042,6 +1103,9 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,6 +1156,12 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1139,6 +1209,12 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1186,6 +1262,9 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1236,6 +1315,12 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1283,6 +1368,12 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1383,6 +1474,12 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1430,6 +1527,12 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1477,6 +1580,9 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1527,6 +1633,12 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1574,6 +1686,12 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1621,6 +1739,9 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1671,6 +1792,12 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1718,6 +1845,12 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>